<commit_message>
Fixed the message layout header for the bytes indicator.
</commit_message>
<xml_diff>
--- a/Docs/Message_Layouts.xlsx
+++ b/Docs/Message_Layouts.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="33">
   <si>
-    <t>BIT</t>
-  </si>
-  <si>
     <t>Bit Number MSB -&gt; LSB</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Ack</t>
+  </si>
+  <si>
+    <t>BYTE</t>
   </si>
 </sst>
 </file>
@@ -364,9 +364,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,6 +416,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,7 +715,7 @@
   <dimension ref="A1:AX27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AZ13" sqref="AZ13"/>
+      <selection activeCell="A17" sqref="A17:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,166 +724,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="K1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="11"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="10"/>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="13"/>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="13"/>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13"/>
-      <c r="AQ2" s="13"/>
-      <c r="AR2" s="13"/>
-      <c r="AS2" s="13"/>
-      <c r="AT2" s="13"/>
-      <c r="AU2" s="13"/>
-      <c r="AV2" s="13"/>
-      <c r="AW2" s="13"/>
-      <c r="AX2" s="14"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="13"/>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13"/>
-      <c r="AI3" s="13"/>
-      <c r="AJ3" s="13"/>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13"/>
-      <c r="AM3" s="13"/>
-      <c r="AN3" s="13"/>
-      <c r="AO3" s="13"/>
-      <c r="AP3" s="13"/>
-      <c r="AQ3" s="13"/>
-      <c r="AR3" s="13"/>
-      <c r="AS3" s="13"/>
-      <c r="AT3" s="13"/>
-      <c r="AU3" s="13"/>
-      <c r="AV3" s="13"/>
-      <c r="AW3" s="13"/>
-      <c r="AX3" s="14"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="12"/>
+      <c r="AO3" s="12"/>
+      <c r="AP3" s="12"/>
+      <c r="AQ3" s="12"/>
+      <c r="AR3" s="12"/>
+      <c r="AS3" s="12"/>
+      <c r="AT3" s="12"/>
+      <c r="AU3" s="12"/>
+      <c r="AV3" s="12"/>
+      <c r="AW3" s="12"/>
+      <c r="AX3" s="13"/>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1">
         <v>7</v>
       </c>
@@ -908,50 +908,50 @@
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="16"/>
-      <c r="AR4" s="16"/>
-      <c r="AS4" s="16"/>
-      <c r="AT4" s="16"/>
-      <c r="AU4" s="16"/>
-      <c r="AV4" s="16"/>
-      <c r="AW4" s="16"/>
-      <c r="AX4" s="17"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
+      <c r="AN4" s="15"/>
+      <c r="AO4" s="15"/>
+      <c r="AP4" s="15"/>
+      <c r="AQ4" s="15"/>
+      <c r="AR4" s="15"/>
+      <c r="AS4" s="15"/>
+      <c r="AT4" s="15"/>
+      <c r="AU4" s="15"/>
+      <c r="AV4" s="15"/>
+      <c r="AW4" s="15"/>
+      <c r="AX4" s="16"/>
     </row>
     <row r="5" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -977,63 +977,63 @@
       <c r="I5" s="5">
         <v>0</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8" t="s">
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8" t="s">
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8" t="s">
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="7"/>
+      <c r="AO5" s="7"/>
+      <c r="AP5" s="7"/>
+      <c r="AQ5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8"/>
-      <c r="AQ5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="8"/>
-      <c r="AT5" s="8"/>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="8"/>
-      <c r="AW5" s="8"/>
-      <c r="AX5" s="8"/>
+      <c r="AR5" s="7"/>
+      <c r="AS5" s="7"/>
+      <c r="AT5" s="7"/>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="7"/>
+      <c r="AW5" s="7"/>
+      <c r="AX5" s="7"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -1041,73 +1041,73 @@
       <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="8"/>
-      <c r="AL6" s="8"/>
-      <c r="AM6" s="8"/>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="8"/>
-      <c r="AP6" s="8"/>
-      <c r="AQ6" s="8"/>
-      <c r="AR6" s="8"/>
-      <c r="AS6" s="8"/>
-      <c r="AT6" s="8"/>
-      <c r="AU6" s="8"/>
-      <c r="AV6" s="8"/>
-      <c r="AW6" s="8"/>
-      <c r="AX6" s="8"/>
+      <c r="D6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="7"/>
+      <c r="AR6" s="7"/>
+      <c r="AS6" s="7"/>
+      <c r="AT6" s="7"/>
+      <c r="AU6" s="7"/>
+      <c r="AV6" s="7"/>
+      <c r="AW6" s="7"/>
+      <c r="AX6" s="7"/>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="19"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="18"/>
       <c r="K7" s="1">
         <v>7</v>
       </c>
@@ -1231,115 +1231,115 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="24"/>
+      <c r="AL8" s="24"/>
+      <c r="AM8" s="24"/>
+      <c r="AN8" s="24"/>
+      <c r="AO8" s="24"/>
+      <c r="AP8" s="24"/>
+      <c r="AQ8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
-      <c r="AM8" s="6"/>
-      <c r="AN8" s="6"/>
-      <c r="AO8" s="6"/>
-      <c r="AP8" s="6"/>
-      <c r="AQ8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR8" s="6"/>
-      <c r="AS8" s="6"/>
-      <c r="AT8" s="6"/>
-      <c r="AU8" s="6"/>
-      <c r="AV8" s="6"/>
-      <c r="AW8" s="6"/>
-      <c r="AX8" s="6"/>
+      <c r="AR8" s="24"/>
+      <c r="AS8" s="24"/>
+      <c r="AT8" s="24"/>
+      <c r="AU8" s="24"/>
+      <c r="AV8" s="24"/>
+      <c r="AW8" s="24"/>
+      <c r="AX8" s="24"/>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="18"/>
+      <c r="K9" s="25" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
@@ -1349,7 +1349,7 @@
       <c r="Q9" s="26"/>
       <c r="R9" s="27"/>
       <c r="S9" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T9" s="26"/>
       <c r="U9" s="26"/>
@@ -1359,7 +1359,7 @@
       <c r="Y9" s="26"/>
       <c r="Z9" s="27"/>
       <c r="AA9" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AB9" s="26"/>
       <c r="AC9" s="26"/>
@@ -1369,7 +1369,7 @@
       <c r="AG9" s="26"/>
       <c r="AH9" s="27"/>
       <c r="AI9" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AJ9" s="26"/>
       <c r="AK9" s="26"/>
@@ -1379,7 +1379,7 @@
       <c r="AO9" s="26"/>
       <c r="AP9" s="27"/>
       <c r="AQ9" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AR9" s="26"/>
       <c r="AS9" s="26"/>
@@ -1391,35 +1391,35 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="18"/>
+      <c r="K10" s="25" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="25" t="s">
-        <v>22</v>
       </c>
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
@@ -1429,7 +1429,7 @@
       <c r="Q10" s="26"/>
       <c r="R10" s="27"/>
       <c r="S10" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T10" s="26"/>
       <c r="U10" s="26"/>
@@ -1439,7 +1439,7 @@
       <c r="Y10" s="26"/>
       <c r="Z10" s="27"/>
       <c r="AA10" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AB10" s="26"/>
       <c r="AC10" s="26"/>
@@ -1449,7 +1449,7 @@
       <c r="AG10" s="26"/>
       <c r="AH10" s="27"/>
       <c r="AI10" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AJ10" s="26"/>
       <c r="AK10" s="26"/>
@@ -1459,7 +1459,7 @@
       <c r="AO10" s="26"/>
       <c r="AP10" s="27"/>
       <c r="AQ10" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AR10" s="26"/>
       <c r="AS10" s="26"/>
@@ -1471,33 +1471,33 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="19"/>
+        <v>14</v>
+      </c>
+      <c r="J11" s="18"/>
       <c r="K11" s="25"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
@@ -1507,7 +1507,7 @@
       <c r="Q11" s="26"/>
       <c r="R11" s="27"/>
       <c r="S11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T11" s="26"/>
       <c r="U11" s="26"/>
@@ -1517,7 +1517,7 @@
       <c r="Y11" s="26"/>
       <c r="Z11" s="27"/>
       <c r="AA11" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB11" s="26"/>
       <c r="AC11" s="26"/>
@@ -1545,33 +1545,33 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="19"/>
+        <v>14</v>
+      </c>
+      <c r="J12" s="18"/>
       <c r="K12" s="25"/>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
@@ -1581,7 +1581,7 @@
       <c r="Q12" s="26"/>
       <c r="R12" s="27"/>
       <c r="S12" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T12" s="26"/>
       <c r="U12" s="26"/>
@@ -1617,33 +1617,33 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="19"/>
+        <v>14</v>
+      </c>
+      <c r="J13" s="18"/>
       <c r="K13" s="25"/>
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -1713,97 +1713,97 @@
       <c r="I14" s="5">
         <v>0</v>
       </c>
-      <c r="J14" s="20"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="11"/>
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="K17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="10"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="14"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="13"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="14"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="13"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="1">
         <v>7</v>
       </c>
@@ -1828,26 +1828,26 @@
       <c r="I20" s="1">
         <v>0</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="17"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="16"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -1873,33 +1873,33 @@
       <c r="I21" s="5">
         <v>0</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -1907,49 +1907,49 @@
       <c r="C22" s="4">
         <v>1</v>
       </c>
-      <c r="D22" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
-      <c r="Z22" s="8"/>
+      <c r="D22" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="19"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="18"/>
       <c r="K23" s="1">
         <v>7</v>
       </c>
@@ -2001,153 +2001,153 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="18"/>
+      <c r="K24" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="24"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="18"/>
+      <c r="K25" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="18"/>
+      <c r="K26" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -2173,10 +2173,51 @@
       <c r="I27" s="5">
         <v>0</v>
       </c>
-      <c r="J27" s="20"/>
+      <c r="J27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:I19"/>
+    <mergeCell ref="K17:Z20"/>
+    <mergeCell ref="J21:J27"/>
+    <mergeCell ref="K21:R22"/>
+    <mergeCell ref="S21:Z22"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="S24:Z24"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="S25:Z25"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="S26:Z26"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="S12:Z12"/>
+    <mergeCell ref="AA12:AH12"/>
+    <mergeCell ref="AI12:AP12"/>
+    <mergeCell ref="AQ12:AX12"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="S13:Z13"/>
+    <mergeCell ref="AA13:AH13"/>
+    <mergeCell ref="AI13:AP13"/>
+    <mergeCell ref="AQ13:AX13"/>
+    <mergeCell ref="AQ11:AX11"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="S10:Z10"/>
+    <mergeCell ref="AA10:AH10"/>
+    <mergeCell ref="AI10:AP10"/>
+    <mergeCell ref="AQ10:AX10"/>
+    <mergeCell ref="AI8:AP8"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="S11:Z11"/>
+    <mergeCell ref="AA11:AH11"/>
+    <mergeCell ref="AI11:AP11"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="S9:Z9"/>
+    <mergeCell ref="AA9:AH9"/>
+    <mergeCell ref="AI9:AP9"/>
+    <mergeCell ref="AQ9:AX9"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:I3"/>
     <mergeCell ref="K1:AX4"/>
@@ -2193,47 +2234,6 @@
     <mergeCell ref="S8:Z8"/>
     <mergeCell ref="AA8:AH8"/>
     <mergeCell ref="AQ8:AX8"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="S9:Z9"/>
-    <mergeCell ref="AA9:AH9"/>
-    <mergeCell ref="AI9:AP9"/>
-    <mergeCell ref="AQ9:AX9"/>
-    <mergeCell ref="AI8:AP8"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="S11:Z11"/>
-    <mergeCell ref="AA11:AH11"/>
-    <mergeCell ref="AI11:AP11"/>
-    <mergeCell ref="AQ11:AX11"/>
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="S10:Z10"/>
-    <mergeCell ref="AA10:AH10"/>
-    <mergeCell ref="AI10:AP10"/>
-    <mergeCell ref="AQ10:AX10"/>
-    <mergeCell ref="K13:R13"/>
-    <mergeCell ref="S13:Z13"/>
-    <mergeCell ref="AA13:AH13"/>
-    <mergeCell ref="AI13:AP13"/>
-    <mergeCell ref="AQ13:AX13"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="S12:Z12"/>
-    <mergeCell ref="AA12:AH12"/>
-    <mergeCell ref="AI12:AP12"/>
-    <mergeCell ref="AQ12:AX12"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:I19"/>
-    <mergeCell ref="K17:Z20"/>
-    <mergeCell ref="J21:J27"/>
-    <mergeCell ref="K21:R22"/>
-    <mergeCell ref="S21:Z22"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="S24:Z24"/>
-    <mergeCell ref="K25:R25"/>
-    <mergeCell ref="S25:Z25"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="S26:Z26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>